<commit_message>
trad pied a coulisse bluetooth fini
</commit_message>
<xml_diff>
--- a/projets/PACBluetooth/20_06_12/premiers pas VBA.xlsx
+++ b/projets/PACBluetooth/20_06_12/premiers pas VBA.xlsx
@@ -1,32 +1,96 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilisateur\Documents\stage\stage_2020_b\projets\PACBluetooth\20_06_12\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB59803D-80F7-456C-B0F2-8511AF8E4881}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <definedNames>
+    <definedName name="ma_plage">Sheet1!$E$5:$G$8</definedName>
+    <definedName name="ma_plage1">Sheet1!$B$2:$G$8</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>é'-;è-</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> à:àà</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> éè:àà</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -é:&amp;"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> èç:é_</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &amp;à':"&amp;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &amp;&amp;:ç-</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &amp;é:-'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &amp;':(ç</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> éè:ç(</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Euclid"/>
     </font>
   </fonts>
   <fills count="2">
@@ -49,8 +113,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +395,179 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A2:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="2" spans="1:4">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1.3999999761581421</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <f xml:space="preserve"> C5+3</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="18">
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="str">
+        <f>trad_PAC_bluetooth(A9)</f>
+        <v xml:space="preserve"> 0,00</v>
+      </c>
+      <c r="C9">
+        <f>B9*2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" ref="B10:B18" si="0">trad_PAC_bluetooth(A10)</f>
+        <v xml:space="preserve"> 0,00</v>
+      </c>
+      <c r="C10">
+        <f t="shared" ref="C10:C14" si="1">B10*2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 0,00</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 0,00</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 27,00</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 62,13</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>124.26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 79,28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 104,31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 11,96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> 12,64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>